<commit_message>
Selenium Assignments : Added few more files
</commit_message>
<xml_diff>
--- a/Selenium-Automation-Elearning-Framework-TestNG/resources/UniformStoreTestSuite.xlsx
+++ b/Selenium-Automation-Elearning-Framework-TestNG/resources/UniformStoreTestSuite.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginSuite" sheetId="1" r:id="rId1"/>
+    <sheet name="RegistrationSuite" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="82">
   <si>
     <t>TESTCASE_ID</t>
   </si>
@@ -70,6 +71,201 @@
   </si>
   <si>
     <t>Pass52</t>
+  </si>
+  <si>
+    <t>UNFTD_003</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>E-Mail</t>
+  </si>
+  <si>
+    <t>Telephone</t>
+  </si>
+  <si>
+    <t>Address 1</t>
+  </si>
+  <si>
+    <t>Address 2</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Password Confirm</t>
+  </si>
+  <si>
+    <t>Test Data 1</t>
+  </si>
+  <si>
+    <t>leena</t>
+  </si>
+  <si>
+    <t>Banashankari</t>
+  </si>
+  <si>
+    <t>bangalore</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Karnataka</t>
+  </si>
+  <si>
+    <t>Test Data 2</t>
+  </si>
+  <si>
+    <t>meera</t>
+  </si>
+  <si>
+    <t>Jayanagar</t>
+  </si>
+  <si>
+    <t>Test Data 3</t>
+  </si>
+  <si>
+    <t>pooja</t>
+  </si>
+  <si>
+    <t>Cyber city</t>
+  </si>
+  <si>
+    <t>chennai</t>
+  </si>
+  <si>
+    <t>Tamil Nadu</t>
+  </si>
+  <si>
+    <t>Test Data 4</t>
+  </si>
+  <si>
+    <t>rohini</t>
+  </si>
+  <si>
+    <t>Gachibowli</t>
+  </si>
+  <si>
+    <t>hyderabad</t>
+  </si>
+  <si>
+    <t>Telangana</t>
+  </si>
+  <si>
+    <t>UNFTD_004</t>
+  </si>
+  <si>
+    <t>rakhi</t>
+  </si>
+  <si>
+    <t>rakhi@gmail.com</t>
+  </si>
+  <si>
+    <t>K.R. Road</t>
+  </si>
+  <si>
+    <t>vaibhavi</t>
+  </si>
+  <si>
+    <t>mathur</t>
+  </si>
+  <si>
+    <t>vaibhav</t>
+  </si>
+  <si>
+    <t>B.T.M layout</t>
+  </si>
+  <si>
+    <t>neethi</t>
+  </si>
+  <si>
+    <t>mohan</t>
+  </si>
+  <si>
+    <t>neethi@gmail.com</t>
+  </si>
+  <si>
+    <t>hgtttww</t>
+  </si>
+  <si>
+    <t>Gokulam</t>
+  </si>
+  <si>
+    <t>Mysore</t>
+  </si>
+  <si>
+    <t>Diya</t>
+  </si>
+  <si>
+    <t>Krishna</t>
+  </si>
+  <si>
+    <t>diya@gmail.com</t>
+  </si>
+  <si>
+    <t>Hitec city</t>
+  </si>
+  <si>
+    <t>diya</t>
+  </si>
+  <si>
+    <t>testcaseid</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>leena2000@gmail.com</t>
+  </si>
+  <si>
+    <t>meera2000@gmail.com</t>
+  </si>
+  <si>
+    <t>pooja2000@gmail.com</t>
+  </si>
+  <si>
+    <t>rohini2000@gmail.com</t>
+  </si>
+  <si>
+    <t>leena2000</t>
+  </si>
+  <si>
+    <t>meera2000</t>
+  </si>
+  <si>
+    <t>pooja2000</t>
+  </si>
+  <si>
+    <t>rohini2000</t>
+  </si>
+  <si>
+    <t>verma2000</t>
+  </si>
+  <si>
+    <t>lakshmi2000</t>
+  </si>
+  <si>
+    <t>nayak2000</t>
+  </si>
+  <si>
+    <t>sharma2000</t>
   </si>
 </sst>
 </file>
@@ -106,7 +302,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -250,12 +446,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -273,6 +514,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -554,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -610,50 +864,504 @@
     </row>
     <row r="3" spans="1:6" ht="25" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="10" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>13</v>
+      <c r="E3" s="9"/>
+      <c r="F3" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="25" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>11</v>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="14" t="s">
+      <c r="E4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="25" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="14" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F4">
-    <sortCondition ref="A2:A4"/>
+  <sortState ref="A2:F5">
+    <sortCondition ref="A2:A5"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
+    <hyperlink ref="C5" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="1">
+        <v>9947472000</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="1">
+        <v>560012</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="1">
+        <v>9876542000</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="1">
+        <v>560089</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="1">
+        <v>7765432000</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="1">
+        <v>687543</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="1">
+        <v>9876502000</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="1">
+        <v>620102</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="1">
+        <v>23456</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="1">
+        <v>9876567738</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="1">
+        <v>560012</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="1">
+        <v>9744666483</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="1">
+        <v>560016</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J8" s="1">
+        <v>571234</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="19">
+        <v>7123457656</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" s="19">
+        <v>9876547</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="M9" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="N9" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E7" r:id="rId6" display="mehadi@gmail.com"/>
+    <hyperlink ref="E8" r:id="rId7"/>
+    <hyperlink ref="E9" r:id="rId8"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Selenium Assessment : Submitted more files
</commit_message>
<xml_diff>
--- a/Selenium-Automation-Elearning-Framework-TestNG/resources/UniformStoreTestSuite.xlsx
+++ b/Selenium-Automation-Elearning-Framework-TestNG/resources/UniformStoreTestSuite.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="LoginSuite" sheetId="1" r:id="rId1"/>
     <sheet name="RegistrationSuite" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="86">
   <si>
     <t>TESTCASE_ID</t>
   </si>
@@ -73,9 +76,6 @@
     <t>Pass52</t>
   </si>
   <si>
-    <t>UNFTD_003</t>
-  </si>
-  <si>
     <t>First Name</t>
   </si>
   <si>
@@ -266,6 +266,21 @@
   </si>
   <si>
     <t>sharma2000</t>
+  </si>
+  <si>
+    <t>fax_num</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>IBM</t>
+  </si>
+  <si>
+    <t>subscribe</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -302,7 +317,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -491,12 +506,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -527,6 +551,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -932,10 +958,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -953,414 +979,586 @@
     <col min="12" max="12" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="P1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="Q1" s="22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="1">
+        <v>23456</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="1">
+        <v>9876567738</v>
+      </c>
+      <c r="G2" s="1">
+        <v>9876567738</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="1">
+        <v>560012</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q2" s="23" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" s="1">
-        <v>9947472000</v>
-      </c>
-      <c r="G2" s="1" t="s">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="1">
+        <v>9744666483</v>
+      </c>
+      <c r="G3" s="1">
+        <v>9744666483</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="K3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="1">
+        <v>560016</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="N3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q3" s="23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L4" s="1">
+        <v>571234</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="1">
-        <v>560012</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>31</v>
+      <c r="N4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" s="23" t="s">
+        <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="1">
-        <v>9876542000</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" s="1" t="s">
+    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="19">
+        <v>7123457656</v>
+      </c>
+      <c r="G5" s="19">
+        <v>7123457656</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" s="19">
+        <v>9876547</v>
+      </c>
+      <c r="M5" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="1">
-        <v>560089</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="1">
-        <v>7765432000</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" s="1">
-        <v>687543</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="F5" s="1">
-        <v>9876502000</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="1" t="s">
+      <c r="N5" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J5" s="1">
-        <v>620102</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="1">
-        <v>23456</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="1">
-        <v>9876567738</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="1">
-        <v>560012</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" s="1">
-        <v>9744666483</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J7" s="1">
-        <v>560016</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="N7" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="J8" s="1">
-        <v>571234</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="N8" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" s="19">
-        <v>7123457656</v>
-      </c>
-      <c r="G9" s="19" t="s">
+      <c r="O5" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="H9" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="I9" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="J9" s="19">
-        <v>9876547</v>
-      </c>
-      <c r="K9" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="L9" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="M9" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="N9" s="21" t="s">
-        <v>67</v>
+      <c r="P5" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q5" s="23" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId2" display="mehadi@gmail.com"/>
     <hyperlink ref="E4" r:id="rId3"/>
     <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E6" r:id="rId5"/>
-    <hyperlink ref="E7" r:id="rId6" display="mehadi@gmail.com"/>
-    <hyperlink ref="E8" r:id="rId7"/>
-    <hyperlink ref="E9" r:id="rId8"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:O1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" customWidth="1"/>
+    <col min="14" max="14" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="1">
+        <v>9947472000</v>
+      </c>
+      <c r="E2" s="1">
+        <v>9947472000</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="1">
+        <v>560012</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="P2" t="str">
+        <f>CONCATENATE("insert into user_account values('",A2,"', '",B2,"', '",C2,"', '",D2,"', '",E2,"', '",F2,"', '",G2,"', '",H2,"', '",I2,"', '",J2,"', '",K2,"', '",L2,"', '",M2,"', '",N2,"', '",O2,"'); ")</f>
+        <v xml:space="preserve">insert into user_account values('leena2000', 'verma2000', 'leena2000@gmail.com', '9947472000', '9947472000', 'IBM', 'Banashankari', 'bangalore', 'bangalore', '560012', 'India', 'Karnataka', 'leena', 'leena', 'No'); </v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="1">
+        <v>9876542000</v>
+      </c>
+      <c r="E3" s="1">
+        <v>9876542000</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="1">
+        <v>560089</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="P3" t="str">
+        <f>CONCATENATE("insert into user_account values('",A3,"', '",B3,"', '",C3,"', '",D3,"', '",E3,"', '",F3,"', '",G3,"', '",H3,"', '",I3,"', '",J3,"', '",K3,"', '",L3,"', '",M3,"', '",N3,"', '",O3,"'); ")</f>
+        <v xml:space="preserve">insert into user_account values('meera2000', 'lakshmi2000', 'meera2000@gmail.com', '9876542000', '9876542000', 'IBM', 'Jayanagar', 'bangalore', 'bangalore', '560089', 'India', 'Karnataka', 'meera', 'meera', 'No'); </v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="1">
+        <v>7765432000</v>
+      </c>
+      <c r="E4" s="1">
+        <v>7765432000</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="1">
+        <v>687543</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="P4" t="str">
+        <f>CONCATENATE("insert into user_account values('",A4,"', '",B4,"', '",C4,"', '",D4,"', '",E4,"', '",F4,"', '",G4,"', '",H4,"', '",I4,"', '",J4,"', '",K4,"', '",L4,"', '",M4,"', '",N4,"', '",O4,"'); ")</f>
+        <v xml:space="preserve">insert into user_account values('pooja2000', 'nayak2000', 'pooja2000@gmail.com', '7765432000', '7765432000', 'IBM', 'Cyber city', 'chennai', 'chennai', '687543', 'India', 'Tamil Nadu', 'pooja', 'pooja', 'No'); </v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="1">
+        <v>9876502000</v>
+      </c>
+      <c r="E5" s="1">
+        <v>9876502000</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="1">
+        <v>620102</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="O5" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="P5" t="str">
+        <f>CONCATENATE("insert into user_account values('",A5,"', '",B5,"', '",C5,"', '",D5,"', '",E5,"', '",F5,"', '",G5,"', '",H5,"', '",I5,"', '",J5,"', '",K5,"', '",L5,"', '",M5,"', '",N5,"', '",O5,"'); ")</f>
+        <v xml:space="preserve">insert into user_account values('rohini2000', 'sharma2000', 'rohini2000@gmail.com', '9876502000', '9876502000', 'IBM', 'Gachibowli', 'hyderabad', 'hyderabad', '620102', 'India', 'Telangana', 'rohini', 'rohini', 'No'); </v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Selenium Assessment : Added new Testcase which verifies data with DB
</commit_message>
<xml_diff>
--- a/Selenium-Automation-Elearning-Framework-TestNG/resources/UniformStoreTestSuite.xlsx
+++ b/Selenium-Automation-Elearning-Framework-TestNG/resources/UniformStoreTestSuite.xlsx
@@ -169,9 +169,6 @@
     <t>Telangana</t>
   </si>
   <si>
-    <t>UNFTD_004</t>
-  </si>
-  <si>
     <t>rakhi</t>
   </si>
   <si>
@@ -281,6 +278,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>UNF_063</t>
   </si>
 </sst>
 </file>
@@ -961,7 +961,7 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -984,10 +984,10 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>17</v>
@@ -1002,10 +1002,10 @@
         <v>20</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>21</v>
@@ -1032,24 +1032,24 @@
         <v>28</v>
       </c>
       <c r="Q1" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1">
         <v>23456</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F2" s="1">
         <v>9876567738</v>
@@ -1058,10 +1058,10 @@
         <v>9876567738</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>32</v>
@@ -1079,30 +1079,30 @@
         <v>34</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q2" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="15" t="s">
         <v>53</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>54</v>
       </c>
       <c r="F3" s="1">
         <v>9744666483</v>
@@ -1111,10 +1111,10 @@
         <v>9744666483</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>32</v>
@@ -1132,48 +1132,48 @@
         <v>34</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q3" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="F4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L4" s="1">
         <v>571234</v>
@@ -1182,33 +1182,33 @@
         <v>33</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q4" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="18" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>43</v>
       </c>
       <c r="C5" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="E5" s="20" t="s">
         <v>63</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>64</v>
       </c>
       <c r="F5" s="19">
         <v>7123457656</v>
@@ -1217,10 +1217,10 @@
         <v>7123457656</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J5" s="19" t="s">
         <v>46</v>
@@ -1238,13 +1238,13 @@
         <v>47</v>
       </c>
       <c r="O5" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P5" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q5" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1316,10 +1316,10 @@
         <v>20</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>21</v>
@@ -1346,18 +1346,18 @@
         <v>28</v>
       </c>
       <c r="O1" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D2" s="1">
         <v>9947472000</v>
@@ -1366,7 +1366,7 @@
         <v>9947472000</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>31</v>
@@ -1393,7 +1393,7 @@
         <v>30</v>
       </c>
       <c r="O2" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P2" t="str">
         <f>CONCATENATE("insert into user_account values('",A2,"', '",B2,"', '",C2,"', '",D2,"', '",E2,"', '",F2,"', '",G2,"', '",H2,"', '",I2,"', '",J2,"', '",K2,"', '",L2,"', '",M2,"', '",N2,"', '",O2,"'); ")</f>
@@ -1402,13 +1402,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" s="1">
         <v>9876542000</v>
@@ -1417,7 +1417,7 @@
         <v>9876542000</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>37</v>
@@ -1444,7 +1444,7 @@
         <v>36</v>
       </c>
       <c r="O3" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P3" t="str">
         <f>CONCATENATE("insert into user_account values('",A3,"', '",B3,"', '",C3,"', '",D3,"', '",E3,"', '",F3,"', '",G3,"', '",H3,"', '",I3,"', '",J3,"', '",K3,"', '",L3,"', '",M3,"', '",N3,"', '",O3,"'); ")</f>
@@ -1453,13 +1453,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="1">
         <v>7765432000</v>
@@ -1468,7 +1468,7 @@
         <v>7765432000</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>40</v>
@@ -1495,7 +1495,7 @@
         <v>39</v>
       </c>
       <c r="O4" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P4" t="str">
         <f>CONCATENATE("insert into user_account values('",A4,"', '",B4,"', '",C4,"', '",D4,"', '",E4,"', '",F4,"', '",G4,"', '",H4,"', '",I4,"', '",J4,"', '",K4,"', '",L4,"', '",M4,"', '",N4,"', '",O4,"'); ")</f>
@@ -1504,13 +1504,13 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" s="1">
         <v>9876502000</v>
@@ -1519,7 +1519,7 @@
         <v>9876502000</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>45</v>
@@ -1546,7 +1546,7 @@
         <v>44</v>
       </c>
       <c r="O5" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P5" t="str">
         <f>CONCATENATE("insert into user_account values('",A5,"', '",B5,"', '",C5,"', '",D5,"', '",E5,"', '",F5,"', '",G5,"', '",H5,"', '",I5,"', '",J5,"', '",K5,"', '",L5,"', '",M5,"', '",N5,"', '",O5,"'); ")</f>

</xml_diff>